<commit_message>
7th to be submit
</commit_message>
<xml_diff>
--- a/individual.xlsx
+++ b/individual.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="174">
   <si>
     <t>GOLD</t>
   </si>
@@ -540,6 +540,15 @@
   </si>
   <si>
     <t>total pred</t>
+  </si>
+  <si>
+    <t>overview</t>
+  </si>
+  <si>
+    <t>totalG</t>
+  </si>
+  <si>
+    <t>totalP</t>
   </si>
 </sst>
 </file>
@@ -995,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2224,6 +2233,18 @@
       <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="F28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>172</v>
+      </c>
       <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -2236,6 +2257,19 @@
       <c r="C29" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f>F8+G9+H10+I11+J12+K13+L14+M15+N16+O17+P18+Q19+R20+S21+T22</f>
+        <v>138</v>
+      </c>
+      <c r="H29">
+        <v>12</v>
+      </c>
+      <c r="I29">
+        <v>150</v>
+      </c>
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
@@ -2248,6 +2282,18 @@
       <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <v>2088</v>
+      </c>
+      <c r="I30">
+        <v>2100</v>
+      </c>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -2259,6 +2305,19 @@
       </c>
       <c r="C31" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="F31" t="s">
+        <v>173</v>
+      </c>
+      <c r="G31">
+        <f>SUM(F23:T23)</f>
+        <v>150</v>
+      </c>
+      <c r="H31">
+        <v>2100</v>
+      </c>
+      <c r="I31">
+        <v>2250</v>
       </c>
       <c r="J31" s="3"/>
     </row>

</xml_diff>